<commit_message>
RESELC into RESELCH and COMH into COMHB
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RCI_Techs.xlsx
+++ b/SubRES_TMPL/SubRes_RCI_Techs.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!Olexandr\ResLab\Modelling\TIMES\TIMES-Shire\SubRES_TMPL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="12585" yWindow="345" windowWidth="7905" windowHeight="9120" tabRatio="727"/>
   </bookViews>
@@ -26,7 +21,7 @@
     <definedName name="VARWSTBO">'[2]O&amp;M waste '!$D$5</definedName>
     <definedName name="VARWSTBP">'[2]O&amp;M waste '!$D$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -36,7 +31,7 @@
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="I10" authorId="0" shapeId="0">
+    <comment ref="I10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="120">
   <si>
     <t>YEAR</t>
   </si>
@@ -385,9 +380,6 @@
     <t>Residential cooling technology  - AC - new 1</t>
   </si>
   <si>
-    <t>RESELC</t>
-  </si>
-  <si>
     <t>RESC</t>
   </si>
   <si>
@@ -406,9 +398,6 @@
     <t>COMELCH</t>
   </si>
   <si>
-    <t>COMH</t>
-  </si>
-  <si>
     <t>COMC</t>
   </si>
   <si>
@@ -428,24 +417,27 @@
   </si>
   <si>
     <t>RESHX</t>
+  </si>
+  <si>
+    <t>COMHB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="11">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-"/>
-    <numFmt numFmtId="168" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="#,##0;\-\ #,##0;_-\ &quot;- &quot;"/>
-    <numFmt numFmtId="170" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-"/>
+    <numFmt numFmtId="169" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="#,##0;\-\ #,##0;_-\ &quot;- &quot;"/>
+    <numFmt numFmtId="171" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="173" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="51" x14ac:knownFonts="1">
     <font>
@@ -1424,17 +1416,17 @@
     <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="36" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="36" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="5">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -1442,318 +1434,318 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="5">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -1761,488 +1753,488 @@
     <xf numFmtId="4" fontId="33" fillId="0" borderId="0" applyBorder="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
@@ -2497,314 +2489,314 @@
     <xf numFmtId="0" fontId="31" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -3314,57 +3306,57 @@
     <xf numFmtId="0" fontId="44" fillId="62" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="45" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="35" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="37" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3372,303 +3364,303 @@
     <xf numFmtId="0" fontId="44" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="55" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="59" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="47" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
@@ -3792,50 +3784,50 @@
     <xf numFmtId="0" fontId="36" fillId="38" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="38" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="38" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -4118,7 +4110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="41" fillId="0" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4157,7 +4149,7 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="41" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -4199,33 +4191,33 @@
     <xf numFmtId="0" fontId="41" fillId="34" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="28" borderId="0" xfId="865" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="3" fillId="26" borderId="13" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="7" fillId="28" borderId="0" xfId="865" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="3" fillId="26" borderId="13" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="29" borderId="12" xfId="865" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="10" fillId="29" borderId="12" xfId="865" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="865" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="10" fillId="29" borderId="14" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="9" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="865" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="10" fillId="29" borderId="14" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="29" borderId="14" xfId="865" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="10" fillId="29" borderId="14" xfId="865" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="8" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="9" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="36" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="36" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="8" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4249,28 +4241,28 @@
     <xf numFmtId="2" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="42" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="42" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="42" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="42" fillId="0" borderId="0" xfId="865" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="862"/>
     <xf numFmtId="0" fontId="41" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="41" fillId="0" borderId="15" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="15" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="862" applyFill="1"/>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="2" fontId="42" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7109,7 +7101,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7144,7 +7136,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7358,35 +7350,35 @@
   </sheetPr>
   <dimension ref="A2:Y84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="19"/>
-    <col min="2" max="2" width="10.73046875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="15.265625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="76.3984375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="15.73046875" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.73046875" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="19"/>
+    <col min="2" max="2" width="10.7109375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.42578125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="19" customWidth="1"/>
-    <col min="8" max="9" width="9.1328125" style="19"/>
-    <col min="10" max="10" width="14.3984375" style="19" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="19"/>
+    <col min="10" max="10" width="14.42578125" style="19" customWidth="1"/>
     <col min="11" max="11" width="10" style="19" customWidth="1"/>
-    <col min="12" max="13" width="9.1328125" style="19"/>
-    <col min="14" max="14" width="9.1328125" style="19" customWidth="1"/>
-    <col min="15" max="19" width="9.1328125" style="19"/>
-    <col min="20" max="20" width="16.3984375" style="19" customWidth="1"/>
-    <col min="21" max="22" width="9.1328125" style="19"/>
-    <col min="23" max="23" width="21.59765625" style="19" customWidth="1"/>
-    <col min="24" max="24" width="9.1328125" style="19"/>
-    <col min="25" max="25" width="18.59765625" style="19" customWidth="1"/>
-    <col min="26" max="26" width="39.73046875" style="19" customWidth="1"/>
-    <col min="27" max="16384" width="9.1328125" style="19"/>
+    <col min="12" max="13" width="9.140625" style="19"/>
+    <col min="14" max="14" width="9.140625" style="19" customWidth="1"/>
+    <col min="15" max="19" width="9.140625" style="19"/>
+    <col min="20" max="20" width="16.42578125" style="19" customWidth="1"/>
+    <col min="21" max="22" width="9.140625" style="19"/>
+    <col min="23" max="23" width="21.5703125" style="19" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="19"/>
+    <col min="25" max="25" width="18.5703125" style="19" customWidth="1"/>
+    <col min="26" max="26" width="39.7109375" style="19" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="2" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G2" s="27" t="s">
         <v>73</v>
       </c>
@@ -7482,7 +7474,7 @@
       <c r="X4" s="8"/>
       <c r="Y4" s="68"/>
     </row>
-    <row r="5" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C5" s="19" t="s">
         <v>55</v>
       </c>
@@ -7524,7 +7516,7 @@
       <c r="X5" s="11"/>
       <c r="Y5" s="69"/>
     </row>
-    <row r="6" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C6" s="19" t="str">
         <f>C41</f>
         <v>RHTNGABN1</v>
@@ -7591,7 +7583,7 @@
       </c>
       <c r="Y6" s="66"/>
     </row>
-    <row r="7" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G7" s="14">
         <v>2020</v>
       </c>
@@ -7633,7 +7625,7 @@
       </c>
       <c r="Y7" s="66"/>
     </row>
-    <row r="8" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G8" s="14">
         <v>2030</v>
       </c>
@@ -7675,7 +7667,7 @@
       </c>
       <c r="Y8" s="66"/>
     </row>
-    <row r="9" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G9" s="14">
         <v>2050</v>
       </c>
@@ -7717,7 +7709,7 @@
       </c>
       <c r="Y9" s="66"/>
     </row>
-    <row r="10" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C10" s="19" t="str">
         <f>C42</f>
         <v>RHTCPWBN1</v>
@@ -7784,7 +7776,7 @@
       </c>
       <c r="Y10" s="66"/>
     </row>
-    <row r="11" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G11" s="16">
         <v>2020</v>
       </c>
@@ -7826,7 +7818,7 @@
       </c>
       <c r="Y11" s="66"/>
     </row>
-    <row r="12" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G12" s="16">
         <v>2030</v>
       </c>
@@ -7868,7 +7860,7 @@
       </c>
       <c r="Y12" s="66"/>
     </row>
-    <row r="13" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G13" s="16">
         <v>2050</v>
       </c>
@@ -7910,7 +7902,7 @@
       </c>
       <c r="Y13" s="66"/>
     </row>
-    <row r="14" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C14" s="19" t="str">
         <f>C43</f>
         <v>RHTELCXN1</v>
@@ -7977,7 +7969,7 @@
       </c>
       <c r="Y14" s="66"/>
     </row>
-    <row r="15" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G15" s="16">
         <v>2020</v>
       </c>
@@ -8019,7 +8011,7 @@
       </c>
       <c r="Y15" s="66"/>
     </row>
-    <row r="16" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G16" s="16">
         <v>2030</v>
       </c>
@@ -8061,7 +8053,7 @@
       </c>
       <c r="Y16" s="66"/>
     </row>
-    <row r="17" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G17" s="16">
         <v>2050</v>
       </c>
@@ -8103,7 +8095,7 @@
       </c>
       <c r="Y17" s="66"/>
     </row>
-    <row r="18" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C18" s="19" t="str">
         <f>C44</f>
         <v>RHTELCXN2</v>
@@ -8173,7 +8165,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="19" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G19" s="16">
         <v>2020</v>
       </c>
@@ -8218,7 +8210,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="20" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G20" s="16">
         <v>2030</v>
       </c>
@@ -8263,7 +8255,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="21" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G21" s="16">
         <v>2050</v>
       </c>
@@ -8308,7 +8300,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="22" spans="3:25" s="72" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:25" s="72" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C22" s="90" t="str">
         <f>C46</f>
         <v>RCTACN1</v>
@@ -8318,10 +8310,10 @@
         <v>Residential cooling technology  - AC - new 1</v>
       </c>
       <c r="E22" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="72" t="s">
         <v>106</v>
-      </c>
-      <c r="F22" s="72" t="s">
-        <v>107</v>
       </c>
       <c r="G22" s="34">
         <v>2015</v>
@@ -8369,7 +8361,7 @@
       <c r="X22" s="34"/>
       <c r="Y22" s="95"/>
     </row>
-    <row r="23" spans="3:25" s="72" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:25" s="72" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G23" s="34">
         <v>2020</v>
       </c>
@@ -8414,7 +8406,7 @@
       <c r="X23" s="34"/>
       <c r="Y23" s="95"/>
     </row>
-    <row r="24" spans="3:25" s="72" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:25" s="72" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G24" s="34">
         <v>2030</v>
       </c>
@@ -8459,7 +8451,7 @@
       <c r="X24" s="34"/>
       <c r="Y24" s="95"/>
     </row>
-    <row r="25" spans="3:25" s="72" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:25" s="72" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G25" s="34">
         <v>2050</v>
       </c>
@@ -8504,7 +8496,7 @@
       <c r="X25" s="34"/>
       <c r="Y25" s="95"/>
     </row>
-    <row r="26" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C26" s="1" t="s">
         <v>81</v>
       </c>
@@ -8526,7 +8518,7 @@
       <c r="U26" s="37"/>
       <c r="X26" s="34"/>
     </row>
-    <row r="27" spans="3:25" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C27" s="13" t="str">
         <f>C45</f>
         <v>RHTHCEBN1</v>
@@ -8539,7 +8531,7 @@
         <v>85</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G27" s="14">
         <v>2012</v>
@@ -8579,7 +8571,7 @@
       </c>
       <c r="X27" s="34"/>
     </row>
-    <row r="28" spans="3:25" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:25" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G28" s="42"/>
       <c r="H28" s="42"/>
       <c r="I28" s="42"/>
@@ -8597,7 +8589,7 @@
       <c r="U28" s="37"/>
       <c r="X28" s="42"/>
     </row>
-    <row r="29" spans="3:25" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:25" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G29" s="42"/>
       <c r="H29" s="42"/>
       <c r="I29" s="42"/>
@@ -8615,7 +8607,7 @@
       <c r="U29" s="37"/>
       <c r="X29" s="42"/>
     </row>
-    <row r="30" spans="3:25" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:25" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G30" s="42"/>
       <c r="H30" s="42"/>
       <c r="I30" s="42"/>
@@ -8633,7 +8625,7 @@
       <c r="U30" s="37"/>
       <c r="X30" s="42"/>
     </row>
-    <row r="31" spans="3:25" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:25" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="F31" s="75"/>
       <c r="G31" s="46"/>
       <c r="K31" s="75"/>
@@ -8649,7 +8641,7 @@
       <c r="U31" s="37"/>
       <c r="X31" s="42"/>
     </row>
-    <row r="32" spans="3:25" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:25" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G32" s="75"/>
       <c r="H32" s="46"/>
       <c r="L32" s="75"/>
@@ -8665,7 +8657,7 @@
       <c r="V32" s="37"/>
       <c r="Y32" s="42"/>
     </row>
-    <row r="33" spans="1:25" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:25" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="H33" s="42"/>
       <c r="I33" s="42"/>
       <c r="J33" s="42"/>
@@ -8683,7 +8675,7 @@
       <c r="V33" s="37"/>
       <c r="Y33" s="42"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C34" s="24"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
@@ -8705,7 +8697,7 @@
       <c r="V34" s="37"/>
       <c r="Y34" s="34"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G35" s="19" t="s">
         <v>84</v>
       </c>
@@ -8726,7 +8718,7 @@
       <c r="V35" s="37"/>
       <c r="Y35" s="34"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="23"/>
       <c r="B38" s="51" t="s">
         <v>72</v>
@@ -8739,7 +8731,7 @@
       <c r="H38" s="52"/>
       <c r="I38" s="52"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="23"/>
       <c r="B39" s="53" t="s">
         <v>71</v>
@@ -8793,7 +8785,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="23"/>
       <c r="B41" s="80" t="s">
         <v>56</v>
@@ -8819,7 +8811,7 @@
       </c>
       <c r="K41" s="88"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="23"/>
       <c r="B42" s="80"/>
       <c r="C42" s="78" t="s">
@@ -8843,7 +8835,7 @@
       </c>
       <c r="K42" s="89"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="23"/>
       <c r="B43" s="80"/>
       <c r="C43" s="78" t="s">
@@ -8867,7 +8859,7 @@
       </c>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="23"/>
       <c r="B44" s="80"/>
       <c r="C44" s="78" t="s">
@@ -8891,7 +8883,7 @@
       </c>
       <c r="K44" s="87"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="23"/>
       <c r="B45" s="80"/>
       <c r="C45" s="80" t="s">
@@ -8915,7 +8907,7 @@
       </c>
       <c r="K45" s="87"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
       <c r="B46" s="80"/>
       <c r="C46" s="78" t="s">
@@ -8939,13 +8931,13 @@
       </c>
       <c r="K46" s="87"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="23"/>
       <c r="B47" s="80"/>
       <c r="K47" s="87"/>
       <c r="L47" s="25"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="23"/>
       <c r="B48" s="55"/>
       <c r="C48" s="55"/>
@@ -8958,7 +8950,7 @@
       <c r="K48" s="87"/>
       <c r="L48" s="25"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
       <c r="B49" s="55"/>
       <c r="C49" s="55"/>
@@ -8971,7 +8963,7 @@
       <c r="K49" s="87"/>
       <c r="L49" s="25"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="25"/>
       <c r="B50" s="57"/>
       <c r="C50" s="55"/>
@@ -8983,7 +8975,7 @@
       <c r="I50" s="52"/>
       <c r="K50" s="87"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="25"/>
       <c r="B51" s="57"/>
       <c r="C51" s="55"/>
@@ -8995,7 +8987,7 @@
       <c r="I51" s="52"/>
       <c r="K51" s="89"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>
       <c r="B52" s="55"/>
       <c r="C52" s="55"/>
@@ -9007,7 +8999,7 @@
       <c r="I52" s="52"/>
       <c r="K52" s="89"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="23"/>
       <c r="B53" s="55"/>
       <c r="C53" s="55"/>
@@ -9019,7 +9011,7 @@
       <c r="I53" s="52"/>
       <c r="K53" s="10"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="23"/>
       <c r="B54" s="24"/>
       <c r="C54" s="23"/>
@@ -9031,7 +9023,7 @@
       <c r="I54" s="26"/>
       <c r="K54" s="87"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
       <c r="B55" s="24"/>
       <c r="C55" s="23"/>
@@ -9043,16 +9035,16 @@
       <c r="I55" s="26"/>
       <c r="K55" s="87"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K56" s="87"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K57" s="87"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K58" s="87"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="58"/>
       <c r="B59" s="58"/>
       <c r="C59" s="59"/>
@@ -9064,7 +9056,7 @@
       <c r="I59" s="59"/>
       <c r="K59" s="87"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="53" t="s">
         <v>52</v>
       </c>
@@ -9093,7 +9085,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="31.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="60" t="s">
         <v>44</v>
       </c>
@@ -9122,7 +9114,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="62" t="s">
         <v>35</v>
       </c>
@@ -9141,7 +9133,7 @@
       <c r="H62" s="55"/>
       <c r="I62" s="55"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="59"/>
       <c r="B63" s="59"/>
       <c r="C63" s="62" t="s">
@@ -9158,7 +9150,7 @@
       <c r="H63" s="59"/>
       <c r="I63" s="59"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="59"/>
       <c r="B64" s="59"/>
       <c r="C64" s="62" t="s">
@@ -9175,7 +9167,7 @@
       <c r="H64" s="59"/>
       <c r="I64" s="59"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="59"/>
       <c r="B65" s="59"/>
       <c r="C65" s="62" t="s">
@@ -9192,7 +9184,7 @@
       <c r="H65" s="59"/>
       <c r="I65" s="59"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="59"/>
       <c r="B66" s="59"/>
       <c r="C66" s="62" t="s">
@@ -9209,7 +9201,7 @@
       <c r="H66" s="59"/>
       <c r="I66" s="59"/>
     </row>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -9224,28 +9216,28 @@
   <dimension ref="A2:V63"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.1328125" style="19"/>
+    <col min="1" max="2" width="9.140625" style="19"/>
     <col min="3" max="3" width="17" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="106.3984375" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.73046875" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1328125" style="19"/>
-    <col min="7" max="7" width="10.59765625" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.1328125" style="19"/>
-    <col min="10" max="10" width="17.3984375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="106.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="19"/>
+    <col min="7" max="7" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="19"/>
+    <col min="10" max="10" width="17.42578125" style="19" customWidth="1"/>
     <col min="11" max="11" width="10" style="19" customWidth="1"/>
-    <col min="12" max="12" width="13.86328125" style="19" customWidth="1"/>
-    <col min="13" max="13" width="10.59765625" style="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.1328125" style="19"/>
-    <col min="16" max="16" width="9.59765625" style="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1328125" style="19"/>
+    <col min="12" max="12" width="13.85546875" style="19" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="19"/>
+    <col min="16" max="16" width="9.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:22" x14ac:dyDescent="0.45">
+    <row r="2" spans="3:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G2" s="27" t="s">
         <v>73</v>
       </c>
@@ -9333,7 +9325,7 @@
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C5" s="19" t="s">
         <v>55</v>
       </c>
@@ -9373,7 +9365,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C6" s="19" t="str">
         <f>C33</f>
         <v>CHTELCXN1</v>
@@ -9383,10 +9375,10 @@
         <v>Commercial heating technology  - direct eletrical heating - new 1</v>
       </c>
       <c r="E6" s="72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F6" s="87" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G6" s="16">
         <v>2015</v>
@@ -9432,7 +9424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G7" s="16">
         <v>2020</v>
       </c>
@@ -9469,7 +9461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G8" s="16">
         <v>2030</v>
       </c>
@@ -9506,7 +9498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G9" s="16">
         <v>2050</v>
       </c>
@@ -9543,7 +9535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C10" s="19" t="str">
         <f>C34</f>
         <v>CHTELCXN2</v>
@@ -9553,10 +9545,10 @@
         <v>Commercial heating technology  - Heat pump, air-to-air - new 2</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F10" s="87" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G10" s="16">
         <v>2015</v>
@@ -9602,7 +9594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G11" s="16">
         <v>2020</v>
       </c>
@@ -9639,7 +9631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G12" s="16">
         <v>2030</v>
       </c>
@@ -9676,7 +9668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G13" s="16">
         <v>2050</v>
       </c>
@@ -9713,7 +9705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:22" s="72" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:22" s="72" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C14" s="90" t="str">
         <f>C36</f>
         <v>CCTACN1</v>
@@ -9723,10 +9715,10 @@
         <v>Commercial cooling technology  - AC - new 1</v>
       </c>
       <c r="E14" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" s="87" t="s">
         <v>112</v>
-      </c>
-      <c r="F14" s="87" t="s">
-        <v>114</v>
       </c>
       <c r="G14" s="34">
         <v>2015</v>
@@ -9772,7 +9764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:22" s="72" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:22" s="72" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G15" s="34">
         <v>2020</v>
       </c>
@@ -9815,7 +9807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="3:22" s="72" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:22" s="72" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G16" s="34">
         <v>2030</v>
       </c>
@@ -9858,7 +9850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="72" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:22" s="72" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G17" s="34">
         <v>2050</v>
       </c>
@@ -9901,7 +9893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C18" s="1" t="s">
         <v>81</v>
       </c>
@@ -9922,7 +9914,7 @@
       <c r="T18" s="47"/>
       <c r="U18" s="47"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C19" s="73" t="str">
         <f>C35</f>
         <v>CHTHCEBN1</v>
@@ -9935,7 +9927,7 @@
         <v>92</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G19" s="14">
         <v>2012</v>
@@ -9974,7 +9966,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:22" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:22" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C20" s="73"/>
       <c r="D20" s="73"/>
       <c r="E20" s="49"/>
@@ -9989,7 +9981,7 @@
       <c r="N20" s="46"/>
       <c r="O20" s="76"/>
     </row>
-    <row r="21" spans="1:22" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:22" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C21" s="73"/>
       <c r="D21" s="73"/>
       <c r="E21" s="49"/>
@@ -10004,7 +9996,7 @@
       <c r="N21" s="46"/>
       <c r="O21" s="76"/>
     </row>
-    <row r="22" spans="1:22" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:22" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C22" s="73"/>
       <c r="D22" s="73"/>
       <c r="J22" s="42"/>
@@ -10012,7 +10004,7 @@
       <c r="L22" s="75"/>
       <c r="M22" s="75"/>
     </row>
-    <row r="23" spans="1:22" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:22" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C23" s="73"/>
       <c r="D23" s="73"/>
       <c r="J23" s="42"/>
@@ -10020,7 +10012,7 @@
       <c r="L23" s="75"/>
       <c r="M23" s="75"/>
     </row>
-    <row r="24" spans="1:22" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:22" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C24" s="73"/>
       <c r="D24" s="73"/>
       <c r="E24" s="75"/>
@@ -10031,7 +10023,7 @@
       <c r="L24" s="75"/>
       <c r="M24" s="75"/>
     </row>
-    <row r="25" spans="1:22" s="74" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:22" s="74" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C25" s="77"/>
       <c r="D25" s="73"/>
       <c r="E25" s="75"/>
@@ -10042,7 +10034,7 @@
       <c r="L25" s="75"/>
       <c r="M25" s="75"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="23"/>
       <c r="B30" s="51" t="s">
         <v>72</v>
@@ -10055,7 +10047,7 @@
       <c r="H30" s="52"/>
       <c r="I30" s="52"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:22" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="23"/>
       <c r="B31" s="53" t="s">
         <v>71</v>
@@ -10082,7 +10074,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="31.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:22" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="23"/>
       <c r="B32" s="54" t="s">
         <v>64</v>
@@ -10109,16 +10101,16 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="23"/>
       <c r="B33" s="80" t="s">
         <v>56</v>
       </c>
       <c r="C33" s="78" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D33" s="78" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E33" s="80" t="s">
         <v>54</v>
@@ -10134,14 +10126,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
       <c r="B34" s="80"/>
       <c r="C34" s="78" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D34" s="78" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E34" s="80" t="s">
         <v>54</v>
@@ -10157,14 +10149,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
       <c r="B35" s="80"/>
       <c r="C35" s="80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D35" s="80" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E35" s="80" t="s">
         <v>54</v>
@@ -10180,14 +10172,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
       <c r="B36" s="80"/>
       <c r="C36" s="78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D36" s="80" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E36" s="80" t="s">
         <v>54</v>
@@ -10203,11 +10195,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
       <c r="B37" s="80"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="23"/>
       <c r="B38" s="80"/>
       <c r="C38" s="78"/>
@@ -10218,13 +10210,13 @@
       <c r="H38" s="79"/>
       <c r="I38" s="79"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="23"/>
       <c r="B39" s="80"/>
       <c r="L39" s="25"/>
       <c r="N39" s="28"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="B40" s="55"/>
       <c r="C40" s="55"/>
@@ -10237,7 +10229,7 @@
       <c r="L40" s="25"/>
       <c r="N40" s="28"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="23"/>
       <c r="B41" s="55"/>
       <c r="C41" s="55"/>
@@ -10250,7 +10242,7 @@
       <c r="L41" s="25"/>
       <c r="N41" s="28"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="23"/>
       <c r="B42" s="55"/>
       <c r="C42" s="86"/>
@@ -10262,7 +10254,7 @@
       <c r="I42" s="52"/>
       <c r="N42" s="28"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="23"/>
       <c r="B43" s="55"/>
       <c r="C43" s="86"/>
@@ -10274,7 +10266,7 @@
       <c r="I43" s="52"/>
       <c r="N43" s="28"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="23"/>
       <c r="B44" s="55"/>
       <c r="C44" s="55"/>
@@ -10286,7 +10278,7 @@
       <c r="I44" s="52"/>
       <c r="N44" s="28"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="23"/>
       <c r="B45" s="55"/>
       <c r="C45" s="55"/>
@@ -10298,7 +10290,7 @@
       <c r="I45" s="52"/>
       <c r="N45" s="28"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
       <c r="B46" s="24"/>
       <c r="C46" s="23"/>
@@ -10310,7 +10302,7 @@
       <c r="I46" s="26"/>
       <c r="N46" s="28"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="23"/>
       <c r="B47" s="24"/>
       <c r="C47" s="23"/>
@@ -10322,7 +10314,7 @@
       <c r="I47" s="26"/>
       <c r="N47" s="28"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="58"/>
       <c r="B51" s="58"/>
       <c r="C51" s="59"/>
@@ -10333,7 +10325,7 @@
       <c r="H51" s="59"/>
       <c r="I51" s="59"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="53" t="s">
         <v>52</v>
       </c>
@@ -10362,7 +10354,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="31.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="60" t="s">
         <v>44</v>
       </c>
@@ -10391,7 +10383,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="62" t="s">
         <v>35</v>
       </c>
@@ -10410,7 +10402,7 @@
       <c r="H54" s="55"/>
       <c r="I54" s="55"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="59"/>
       <c r="B55" s="59"/>
       <c r="C55" s="62" t="s">
@@ -10427,7 +10419,7 @@
       <c r="H55" s="59"/>
       <c r="I55" s="59"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="59"/>
       <c r="B56" s="59"/>
       <c r="C56" s="62" t="s">
@@ -10444,7 +10436,7 @@
       <c r="H56" s="59"/>
       <c r="I56" s="59"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="59"/>
       <c r="B57" s="59"/>
       <c r="C57" s="62" t="s">
@@ -10461,7 +10453,7 @@
       <c r="H57" s="59"/>
       <c r="I57" s="59"/>
     </row>
-    <row r="58" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="59"/>
       <c r="B58" s="59"/>
       <c r="C58" s="62" t="s">
@@ -10478,10 +10470,10 @@
       <c r="H58" s="59"/>
       <c r="I58" s="59"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C62" s="40"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C63" s="40"/>
     </row>
   </sheetData>
@@ -10502,25 +10494,25 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.1328125" style="72"/>
+    <col min="1" max="2" width="9.140625" style="72"/>
     <col min="3" max="3" width="17" style="72" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="106.3984375" style="72" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.73046875" style="72" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1328125" style="72"/>
-    <col min="7" max="7" width="10.59765625" style="72" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.1328125" style="72"/>
-    <col min="10" max="10" width="17.3984375" style="72" customWidth="1"/>
+    <col min="4" max="4" width="106.42578125" style="72" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="72" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="72"/>
+    <col min="7" max="7" width="10.5703125" style="72" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="72"/>
+    <col min="10" max="10" width="17.42578125" style="72" customWidth="1"/>
     <col min="11" max="11" width="10" style="72" customWidth="1"/>
-    <col min="12" max="12" width="13.86328125" style="72" customWidth="1"/>
-    <col min="13" max="13" width="10.59765625" style="72" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.1328125" style="72"/>
-    <col min="16" max="16" width="9.59765625" style="72" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1328125" style="72"/>
+    <col min="12" max="12" width="13.85546875" style="72" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="72" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="72"/>
+    <col min="16" max="16" width="9.5703125" style="72" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="72"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G2" s="27" t="s">
         <v>73</v>
       </c>
@@ -10605,7 +10597,7 @@
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C5" s="72" t="s">
         <v>55</v>
       </c>
@@ -10645,7 +10637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C6" s="72" t="s">
         <v>89</v>
       </c>
@@ -10702,7 +10694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G7" s="14">
         <v>2020</v>
       </c>
@@ -10739,7 +10731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="E8" s="28"/>
       <c r="F8" s="28"/>
       <c r="G8" s="14">
@@ -10778,7 +10770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G9" s="14">
         <v>2050</v>
       </c>
@@ -10815,7 +10807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="23"/>
       <c r="B12" s="51" t="s">
         <v>72</v>
@@ -10828,7 +10820,7 @@
       <c r="H12" s="52"/>
       <c r="I12" s="52"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="23"/>
       <c r="B13" s="53" t="s">
         <v>71</v>
@@ -10882,7 +10874,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="23"/>
       <c r="B15" s="80" t="s">
         <v>56</v>
@@ -10907,7 +10899,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="23"/>
       <c r="B16" s="80"/>
       <c r="C16" s="78"/>
@@ -10918,7 +10910,7 @@
       <c r="H16" s="79"/>
       <c r="I16" s="79"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="23"/>
       <c r="B17" s="80"/>
       <c r="C17" s="78"/>
@@ -10929,7 +10921,7 @@
       <c r="H17" s="79"/>
       <c r="I17" s="79"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="23"/>
       <c r="B18" s="80"/>
       <c r="C18" s="78"/>
@@ -10940,7 +10932,7 @@
       <c r="H18" s="79"/>
       <c r="I18" s="79"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="23"/>
       <c r="B19" s="80"/>
       <c r="C19" s="78"/>
@@ -10951,7 +10943,7 @@
       <c r="H19" s="79"/>
       <c r="I19" s="79"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="23"/>
       <c r="B20" s="80"/>
       <c r="C20" s="80"/>
@@ -10965,7 +10957,7 @@
       <c r="L20" s="25"/>
       <c r="N20" s="28"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="23"/>
       <c r="B21" s="55"/>
       <c r="C21" s="55"/>
@@ -10979,7 +10971,7 @@
       <c r="L21" s="25"/>
       <c r="N21" s="28"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="23"/>
       <c r="B22" s="55"/>
       <c r="C22" s="55"/>
@@ -10993,7 +10985,7 @@
       <c r="L22" s="25"/>
       <c r="N22" s="28"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="23"/>
       <c r="B23" s="55"/>
       <c r="C23" s="86"/>
@@ -11005,7 +10997,7 @@
       <c r="I23" s="52"/>
       <c r="N23" s="28"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="23"/>
       <c r="B24" s="55"/>
       <c r="C24" s="86"/>
@@ -11017,7 +11009,7 @@
       <c r="I24" s="52"/>
       <c r="N24" s="28"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="23"/>
       <c r="B25" s="55"/>
       <c r="C25" s="55"/>
@@ -11029,7 +11021,7 @@
       <c r="I25" s="52"/>
       <c r="N25" s="28"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="23"/>
       <c r="B26" s="55"/>
       <c r="C26" s="55"/>
@@ -11041,7 +11033,7 @@
       <c r="I26" s="52"/>
       <c r="N26" s="28"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="23"/>
       <c r="B27" s="24"/>
       <c r="C27" s="23"/>
@@ -11053,7 +11045,7 @@
       <c r="I27" s="26"/>
       <c r="N27" s="28"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="23"/>
       <c r="B28" s="24"/>
       <c r="C28" s="23"/>
@@ -11065,7 +11057,7 @@
       <c r="I28" s="26"/>
       <c r="N28" s="28"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="58"/>
       <c r="B32" s="58"/>
       <c r="C32" s="59"/>
@@ -11076,7 +11068,7 @@
       <c r="H32" s="59"/>
       <c r="I32" s="59"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="53" t="s">
         <v>52</v>
       </c>
@@ -11105,7 +11097,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="31.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="60" t="s">
         <v>44</v>
       </c>
@@ -11134,7 +11126,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="62" t="s">
         <v>35</v>
       </c>
@@ -11153,7 +11145,7 @@
       <c r="H35" s="55"/>
       <c r="I35" s="55"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="59"/>
       <c r="B36" s="59"/>
       <c r="C36" s="62" t="s">
@@ -11170,7 +11162,7 @@
       <c r="H36" s="59"/>
       <c r="I36" s="59"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="59"/>
       <c r="B37" s="59"/>
       <c r="C37" s="62" t="s">
@@ -11187,7 +11179,7 @@
       <c r="H37" s="59"/>
       <c r="I37" s="59"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="59"/>
       <c r="B38" s="59"/>
       <c r="C38" s="62" t="s">
@@ -11204,7 +11196,7 @@
       <c r="H38" s="59"/>
       <c r="I38" s="59"/>
     </row>
-    <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="59"/>
       <c r="B39" s="59"/>
       <c r="C39" s="62" t="s">
@@ -11221,10 +11213,10 @@
       <c r="H39" s="59"/>
       <c r="I39" s="59"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C43" s="40"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C44" s="40"/>
     </row>
   </sheetData>
@@ -11234,26 +11226,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Phase xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">
-      <Value>Contracted</Value>
-    </Phase>
-    <PortalAuthor xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="File" ma:contentTypeID="0x0101000DD098BE9899426A8B0406C5EF9CA50A0088BDD742C1DD304A87D731357DBB47E2" ma:contentTypeVersion="1" ma:contentTypeDescription="This is the base type for all file formats" ma:contentTypeScope="" ma:versionID="7ff74889935fc138bd7541b24877147a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46dc3d67e2c7a72f7fde2a6a9b1bcac1" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -11335,31 +11307,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE784753-1928-4D6F-83BC-1FAE29BA76C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5848600-2E8A-4836-874B-3D5E5B443EC6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Phase xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">
+      <Value>Contracted</Value>
+    </Phase>
+    <PortalAuthor xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5D6C50A-3B64-4A50-9420-90562322C579}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11374,4 +11342,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5848600-2E8A-4836-874B-3D5E5B443EC6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE784753-1928-4D6F-83BC-1FAE29BA76C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>